<commit_message>
updates for nfl 2020
</commit_message>
<xml_diff>
--- a/data-raw/db_sports.xlsx
+++ b/data-raw/db_sports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aelhabr\Documents\projects\sports-predict\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C444BBED-BF14-4754-81FA-160AFE5176EA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045810A7-EE5D-43BC-BAE3-0CB89668CFE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3375" yWindow="1275" windowWidth="25425" windowHeight="14925" tabRatio="730" activeTab="1" xr2:uid="{F299F711-D4F9-455C-93CD-33799F69C1A9}"/>
+    <workbookView xWindow="3810" yWindow="3810" windowWidth="13485" windowHeight="11520" tabRatio="730" activeTab="1" xr2:uid="{F299F711-D4F9-455C-93CD-33799F69C1A9}"/>
   </bookViews>
   <sheets>
     <sheet name="nfl_tm" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="192">
   <si>
     <t>game_result_id</t>
   </si>
@@ -599,6 +599,18 @@
   </si>
   <si>
     <t>WSH</t>
+  </si>
+  <si>
+    <t>LVR</t>
+  </si>
+  <si>
+    <t>Las Vegas Raiders</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
+  </si>
+  <si>
+    <t>LAV</t>
   </si>
 </sst>
 </file>
@@ -950,11 +962,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3B3ECA7-9A25-40A8-9453-2E882EECF8B1}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1551,7 +1566,7 @@
         <v>92</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1782,6 +1797,29 @@
       </c>
       <c r="G36">
         <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>188</v>
+      </c>
+      <c r="C37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D37" t="s">
+        <v>190</v>
+      </c>
+      <c r="E37" t="s">
+        <v>191</v>
+      </c>
+      <c r="F37" t="s">
+        <v>189</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1792,9 +1830,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87E0B7D-391B-47A1-BFA0-908005119D46}">
-  <dimension ref="A1:G257"/>
+  <dimension ref="A1:G273"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
+      <selection activeCell="F266" sqref="F266"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -7707,6 +7747,374 @@
       </c>
       <c r="G257" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>2116</v>
+      </c>
+      <c r="B258">
+        <v>1</v>
+      </c>
+      <c r="C258">
+        <v>2020</v>
+      </c>
+      <c r="D258">
+        <v>1</v>
+      </c>
+      <c r="E258">
+        <v>1</v>
+      </c>
+      <c r="F258" t="s">
+        <v>20</v>
+      </c>
+      <c r="G258" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>2117</v>
+      </c>
+      <c r="B259">
+        <v>1</v>
+      </c>
+      <c r="C259">
+        <v>2020</v>
+      </c>
+      <c r="D259">
+        <v>1</v>
+      </c>
+      <c r="E259">
+        <v>1</v>
+      </c>
+      <c r="F259" t="s">
+        <v>30</v>
+      </c>
+      <c r="G259" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>2118</v>
+      </c>
+      <c r="B260">
+        <v>1</v>
+      </c>
+      <c r="C260">
+        <v>2020</v>
+      </c>
+      <c r="D260">
+        <v>1</v>
+      </c>
+      <c r="E260">
+        <v>1</v>
+      </c>
+      <c r="F260" t="s">
+        <v>36</v>
+      </c>
+      <c r="G260" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>2119</v>
+      </c>
+      <c r="B261">
+        <v>1</v>
+      </c>
+      <c r="C261">
+        <v>2020</v>
+      </c>
+      <c r="D261">
+        <v>1</v>
+      </c>
+      <c r="E261">
+        <v>1</v>
+      </c>
+      <c r="F261" t="s">
+        <v>34</v>
+      </c>
+      <c r="G261" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>2120</v>
+      </c>
+      <c r="B262">
+        <v>1</v>
+      </c>
+      <c r="C262">
+        <v>2020</v>
+      </c>
+      <c r="D262">
+        <v>1</v>
+      </c>
+      <c r="E262">
+        <v>1</v>
+      </c>
+      <c r="F262" t="s">
+        <v>9</v>
+      </c>
+      <c r="G262" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>2121</v>
+      </c>
+      <c r="B263">
+        <v>1</v>
+      </c>
+      <c r="C263">
+        <v>2020</v>
+      </c>
+      <c r="D263">
+        <v>1</v>
+      </c>
+      <c r="E263">
+        <v>1</v>
+      </c>
+      <c r="F263" t="s">
+        <v>33</v>
+      </c>
+      <c r="G263" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>2122</v>
+      </c>
+      <c r="B264">
+        <v>1</v>
+      </c>
+      <c r="C264">
+        <v>2020</v>
+      </c>
+      <c r="D264">
+        <v>1</v>
+      </c>
+      <c r="E264">
+        <v>1</v>
+      </c>
+      <c r="F264" t="s">
+        <v>11</v>
+      </c>
+      <c r="G264" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>2123</v>
+      </c>
+      <c r="B265">
+        <v>1</v>
+      </c>
+      <c r="C265">
+        <v>2020</v>
+      </c>
+      <c r="D265">
+        <v>1</v>
+      </c>
+      <c r="E265">
+        <v>1</v>
+      </c>
+      <c r="F265" t="s">
+        <v>191</v>
+      </c>
+      <c r="G265" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>2124</v>
+      </c>
+      <c r="B266">
+        <v>1</v>
+      </c>
+      <c r="C266">
+        <v>2020</v>
+      </c>
+      <c r="D266">
+        <v>1</v>
+      </c>
+      <c r="E266">
+        <v>1</v>
+      </c>
+      <c r="F266" t="s">
+        <v>13</v>
+      </c>
+      <c r="G266" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>2125</v>
+      </c>
+      <c r="B267">
+        <v>1</v>
+      </c>
+      <c r="C267">
+        <v>2020</v>
+      </c>
+      <c r="D267">
+        <v>1</v>
+      </c>
+      <c r="E267">
+        <v>1</v>
+      </c>
+      <c r="F267" t="s">
+        <v>7</v>
+      </c>
+      <c r="G267" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>2126</v>
+      </c>
+      <c r="B268">
+        <v>1</v>
+      </c>
+      <c r="C268">
+        <v>2020</v>
+      </c>
+      <c r="D268">
+        <v>1</v>
+      </c>
+      <c r="E268">
+        <v>1</v>
+      </c>
+      <c r="F268" t="s">
+        <v>25</v>
+      </c>
+      <c r="G268" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>2127</v>
+      </c>
+      <c r="B269">
+        <v>1</v>
+      </c>
+      <c r="C269">
+        <v>2020</v>
+      </c>
+      <c r="D269">
+        <v>1</v>
+      </c>
+      <c r="E269">
+        <v>1</v>
+      </c>
+      <c r="F269" t="s">
+        <v>24</v>
+      </c>
+      <c r="G269" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>2128</v>
+      </c>
+      <c r="B270">
+        <v>1</v>
+      </c>
+      <c r="C270">
+        <v>2020</v>
+      </c>
+      <c r="D270">
+        <v>1</v>
+      </c>
+      <c r="E270">
+        <v>1</v>
+      </c>
+      <c r="F270" t="s">
+        <v>27</v>
+      </c>
+      <c r="G270" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>2129</v>
+      </c>
+      <c r="B271">
+        <v>1</v>
+      </c>
+      <c r="C271">
+        <v>2020</v>
+      </c>
+      <c r="D271">
+        <v>1</v>
+      </c>
+      <c r="E271">
+        <v>1</v>
+      </c>
+      <c r="F271" t="s">
+        <v>32</v>
+      </c>
+      <c r="G271" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>2130</v>
+      </c>
+      <c r="B272">
+        <v>1</v>
+      </c>
+      <c r="C272">
+        <v>2020</v>
+      </c>
+      <c r="D272">
+        <v>1</v>
+      </c>
+      <c r="E272">
+        <v>1</v>
+      </c>
+      <c r="F272" t="s">
+        <v>10</v>
+      </c>
+      <c r="G272" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>2131</v>
+      </c>
+      <c r="B273">
+        <v>1</v>
+      </c>
+      <c r="C273">
+        <v>2020</v>
+      </c>
+      <c r="D273">
+        <v>1</v>
+      </c>
+      <c r="E273">
+        <v>1</v>
+      </c>
+      <c r="F273" t="s">
+        <v>14</v>
+      </c>
+      <c r="G273" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>